<commit_message>
linkedlist module is done,and pushed few changes in other pages too
</commit_message>
<xml_diff>
--- a/src/test/resources/configfiles/ExcelData.xlsx
+++ b/src/test/resources/configfiles/ExcelData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="signindata" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t xml:space="preserve">username</t>
   </si>
@@ -71,86 +71,34 @@
     <t xml:space="preserve">hello</t>
   </si>
   <si>
-    <t xml:space="preserve">def search(input_list, num):
-	if(num in input_list):
-		print("Element Found")
-	else:
-		print("Not Found")
-Search([12, 23, 45, 67, 6, 90] , 12)
-</t>
+    <t xml:space="preserve">print("welcome)”;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SyntaxError: bad input on line 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def search(lst,value):
+if(value in lst):
+return "Element Found"
+else:
+return "Not Found"
+pass
+print(search([1,2,3],1))</t>
   </si>
   <si>
     <t xml:space="preserve">Element Found</t>
   </si>
   <si>
-    <t xml:space="preserve">def search(input_list, num):
-  if(num in input_list):
-    print("Element Found")
-    \b
-    \b
-   else:
-     print("Not Found")
-     \b
-     \b
-     \b
-     \b
-Search([12, 23, 45, 67, 6, 90] , 12)</t>
+    <t xml:space="preserve">print hello</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NameError: name 'hello' is not defined on line 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
   </si>
   <si>
     <t xml:space="preserve">submission success</t>
-  </si>
-  <si>
-    <t xml:space="preserve">def findMaxConsecutiveOnes(nums) :
-count = 0
-result = 0
-for i in range(0, len(nums)):
-if (nums[i] == 0):
-count = 0
-\b
-\b
-else:
-count+= 1
-\b
-\b
-result = max(result, count)
-\b
-\b
-print(result)
-\b
-\b
-findMaxConsecutiveOnes([1,0,1,1,0,1])</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">def findNumbers(nums):
-c=0
-for i in nums:
-j=str(i)
-x=len(j)
-if x%2==0:
-c=c+1
-\b
-\b
-\b
-\b
-print c
-return c
-findNumbers([12,345,2,6,7896])</t>
-  </si>
-  <si>
-    <t xml:space="preserve">def sortedSquares(nums):
-squares_list = []
-for i in range(0, len(nums)):
-square = nums[i] * nums[i];
-squares_list.append(square)
-\b
-\b
-sorted_squares_list = sorted(squares_list)
-print sorted_squares_list;
-return sorted_squares_list;
-sortedSquares([-7,-3,2,3,11])</t>
   </si>
   <si>
     <t xml:space="preserve">[4, 9, 9, 49, 121]</t>
@@ -272,16 +220,16 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="4" style="0" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="4" style="0" width="8.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -357,11 +305,11 @@
   </sheetPr>
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.43"/>
   </cols>
@@ -374,7 +322,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -384,74 +332,62 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="256.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>20</v>
-      </c>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2"/>
       <c r="B6" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="256.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>20</v>
-      </c>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2"/>
       <c r="B7" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2"/>
+      <c r="B8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="9" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="A9" s="2"/>
       <c r="B9" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="A10" s="2"/>
       <c r="B10" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="2"/>
+      <c r="B11" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data structures module is completed.changes in home page too
</commit_message>
<xml_diff>
--- a/src/test/resources/configfiles/ExcelData.xlsx
+++ b/src/test/resources/configfiles/ExcelData.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="signindata" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="linkedList" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="DataStructures" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t xml:space="preserve">username</t>
   </si>
@@ -102,6 +103,9 @@
   </si>
   <si>
     <t xml:space="preserve">[4, 9, 9, 49, 121]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pythoncode</t>
   </si>
 </sst>
 </file>
@@ -112,7 +116,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -134,6 +138,38 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -184,7 +220,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -199,6 +235,26 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -224,7 +280,7 @@
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.45703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.71"/>
@@ -305,11 +361,11 @@
   </sheetPr>
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.45703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.43"/>
   </cols>
@@ -399,4 +455,64 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.29"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="119.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding test scenarios for array moduel and other changes
</commit_message>
<xml_diff>
--- a/src/test/resources/configfiles/ExcelData.xlsx
+++ b/src/test/resources/configfiles/ExcelData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Tree" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,6 +16,7 @@
     <sheet name="DataStructures" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="Graph" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="Queue" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="homepage" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="47">
   <si>
     <t xml:space="preserve">pythonCode</t>
   </si>
@@ -60,7 +61,7 @@
 return "Element Found"
 else:
 return "Not Found"
-Pass
+pass
 </t>
     </r>
     <r>
@@ -138,63 +139,137 @@
     <t xml:space="preserve">[4, 9, 9, 49, 121]</t>
   </si>
   <si>
+    <t xml:space="preserve">Submission Successful</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def findMaxConsecutiveOnes(nums) :
+count = 0
+result = 0
+for i in range(0, len(nums)):
+if (nums[i] == 0):
+count = 0
+pass
+else:
+count+= 1
+pass
+result = max(result, count)
+pass
+print(result)
+pass
+pass
+findMaxConsecutiveOnes([1,0,1,1,0,1])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def findMaxConsecutiveOnes(nums) :
+count = 0
+result = 0
+for i in range(0, len(nums)):
+if (nums[i] == 0):
+count = 0
+pass
+else:
+count+= 1
+result = max(result, count)
+pass
+pass
+return result
+pass
+findMaxConsecutiveOnes([1,0,1,1,0,1])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def findNumbers(nums):
+c=0
+for i in nums:
+j=str(i)
+x=len(j)
+if x%2==0:
+c=c+1
+pass
+print c
+return c
+pass
+findNumbers([12,345,2,6,7896])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def findNumbers(nums):
+c=0
+for i in nums:
+j=str(i)
+x=len(j)
+if x%2==0:
+c=c+1
+pass
+pass
+return c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def sortedSquares(nums):
+squares_list = []
+for i in range(0, len(nums)):
+square = nums[i] * nums[i];
+squares_list.append(square)
+sorted_squares_list = sorted(squares_list)
+pass
+print(sorted_squares_list)
+return sorted_squares_list
+pass
+sortedSquares([-4,-1,0,3,10])
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0, 1, 9, 16, 100]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def sortedSquares(nums):
+squares_list = []
+for i in range(0, len(nums)):
+square = nums[i] * nums[i];
+squares_list.append(square)
+sorted_squares_list = sorted(squares_list)
+pass
+return sorted_squares_list
+pass
+sortedSquares([-4,-1,0,3,10])
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> No tests were collected</t>
+  </si>
+  <si>
     <t xml:space="preserve">pythoncode</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">def search(lst,value):
-if(value in lst):
-return "Element Found"
-else:
-return "Not Found"
-pass
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Print(search([1,2,3],1))</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">def search(lst,value):
-if(value in lst):
-return "Element Found"
-else:
-return "Not Found"
-pass
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">print(search([1,2,3],1))</t>
-    </r>
+    <t xml:space="preserve">options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">getStartedOptions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arrays</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DataStructures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linkedlist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Queue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Graph</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -351,10 +426,10 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50.57"/>
@@ -422,12 +497,12 @@
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="4" style="0" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="4" style="0" width="8.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -507,7 +582,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.43"/>
   </cols>
@@ -610,7 +685,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.57"/>
@@ -708,13 +783,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.57"/>
@@ -760,40 +835,60 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5" t="s">
+    <row r="6" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="216.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4"/>
+    <row r="8" customFormat="false" ht="203.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="B8" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="163.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="B9" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="136.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="B10" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="B11" s="5" t="s">
-        <v>24</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="163.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -818,15 +913,15 @@
       <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.3"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -872,13 +967,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50.57"/>
@@ -886,7 +981,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -910,7 +1005,7 @@
     </row>
     <row r="4" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
@@ -922,6 +1017,14 @@
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -946,7 +1049,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50.57"/>
@@ -978,7 +1081,7 @@
     </row>
     <row r="4" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
@@ -990,6 +1093,97 @@
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.11"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>